<commit_message>
Analisis y graficos de estadisticas, falta regulares
</commit_message>
<xml_diff>
--- a/Documentacion/GraficosGrafos.xlsx
+++ b/Documentacion/GraficosGrafos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Numero de corridas minimo" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +151,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBE4D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -353,11 +359,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,9 +406,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -435,7 +466,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +585,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$B$45</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$B$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -565,112 +614,130 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$46:$A$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>193</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>194</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>195</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>197</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>198</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>199</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>202</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>203</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>205</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>206</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>207</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>209</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>211</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>212</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>215</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>216</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>217</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>218</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>219</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>221</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$B$46:$B$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$B$45:$B$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -678,73 +745,73 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1142</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1525</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1485</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>842</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>134</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>261</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>507</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>883</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1210</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1471</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1532</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1369</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1090</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -762,6 +829,24 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -779,7 +864,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$C$45</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$C$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -808,165 +893,183 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$46:$A$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>193</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>194</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>195</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>197</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>198</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>199</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>202</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>203</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>205</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>206</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>207</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>209</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>211</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>212</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>215</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>216</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>217</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>218</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>219</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>221</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$C$46:$C$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$C$45:$C$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1166</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1628</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1690</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>177</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>494</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>983</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1487</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1812</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1846</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1463</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>940</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>445</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1005,6 +1108,24 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1022,7 +1143,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$D$45</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$D$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1051,112 +1172,130 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$46:$A$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>193</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>194</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>195</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>196</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>197</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>198</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>199</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>202</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>203</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>205</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>206</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>207</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>209</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>211</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>212</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>213</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>215</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>216</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>217</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>218</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>219</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>221</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$D$46:$D$76</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$D$45:$D$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1194,61 +1333,79 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>58</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>95</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>278</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>527</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>893</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1226</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1582</c:v>
+                  <c:v>356</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1581</c:v>
+                  <c:v>636</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1445</c:v>
+                  <c:v>1034</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1017</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>665</c:v>
+                  <c:v>1557</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>380</c:v>
+                  <c:v>1531</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>156</c:v>
+                  <c:v>1214</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53</c:v>
+                  <c:v>939</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>19</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6</c:v>
+                  <c:v>331</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,6 +1436,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> de colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1344,6 +1561,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Freciencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1381,7 +1654,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1537,7 +1810,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$B$22</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1566,10 +1839,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$23:$A$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$22:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>95</c:v>
                 </c:pt>
@@ -1626,19 +1899,16 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$B$23:$B$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$B$22:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1649,43 +1919,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>774</c:v>
+                  <c:v>749</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1706</c:v>
+                  <c:v>1718</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2571</c:v>
+                  <c:v>2599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2442</c:v>
+                  <c:v>2412</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1473</c:v>
+                  <c:v>1481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>610</c:v>
+                  <c:v>614</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1694,9 +1964,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1714,7 +1981,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$C$22</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1743,10 +2010,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$23:$A$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$22:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>95</c:v>
                 </c:pt>
@@ -1803,48 +2070,45 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$C$23:$C$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$C$22:$C$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>308</c:v>
+                  <c:v>348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1212</c:v>
+                  <c:v>1165</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2565</c:v>
+                  <c:v>2549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3046</c:v>
+                  <c:v>2899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1908</c:v>
+                  <c:v>2014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>742</c:v>
+                  <c:v>761</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>152</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
@@ -1865,15 +2129,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1891,7 +2146,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Numero de corridas minimo'!$D$22</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$D$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1920,10 +2175,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$A$23:$A$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$A$22:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>95</c:v>
                 </c:pt>
@@ -1980,19 +2235,16 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Numero de corridas minimo'!$D$23:$D$42</c:f>
+              <c:f>'[1]Graficos con porcentajes'!$D$22:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2012,46 +2264,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1572</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2377</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1639</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>792</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>185</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>726</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1563</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2396</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2474</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1592</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>742</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2082,6 +2331,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> de colores</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2147,6 +2457,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3464,7 +3830,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-097D-4772-93B2-3B5BB79F93E4}"/>
+              <c16:uniqueId val="{00000000-0262-47C2-AE41-A58F8FB31FE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3617,7 +3983,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-097D-4772-93B2-3B5BB79F93E4}"/>
+              <c16:uniqueId val="{00000001-0262-47C2-AE41-A58F8FB31FE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3770,7 +4136,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-097D-4772-93B2-3B5BB79F93E4}"/>
+              <c16:uniqueId val="{00000002-0262-47C2-AE41-A58F8FB31FE7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3783,16 +4149,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="543398207"/>
-        <c:axId val="543393215"/>
+        <c:axId val="1801188207"/>
+        <c:axId val="1801189871"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="543398207"/>
+        <c:axId val="1801188207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> de colores</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3830,7 +4257,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543393215"/>
+        <c:crossAx val="1801189871"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3838,7 +4265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="543393215"/>
+        <c:axId val="1801189871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3858,6 +4285,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3889,7 +4372,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543398207"/>
+        <c:crossAx val="1801188207"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6714,13 +7197,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>410936</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>83684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6752,13 +7235,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>349702</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>21772</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6790,13 +7273,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>72118</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6828,13 +7311,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>167368</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>53068</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6865,28 +7348,20 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>504265</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:colOff>273323</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>86139</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>392206</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>554932</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>162339</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Gráfico 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6909,6 +7384,7 @@
     <sheetNames>
       <sheetName val="Graficos con porcentajes"/>
       <sheetName val="Numero de corrida minimo"/>
+      <sheetName val="Numero de corridas minimo"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -8151,6 +8627,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8419,27 +8896,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -8465,7 +8942,7 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="37">
         <v>0</v>
       </c>
     </row>
@@ -8479,7 +8956,7 @@
       <c r="C4" s="5">
         <v>52</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="37">
         <v>0</v>
       </c>
     </row>
@@ -8493,7 +8970,7 @@
       <c r="C5" s="5">
         <v>647</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="37">
         <v>0</v>
       </c>
     </row>
@@ -8507,7 +8984,7 @@
       <c r="C6" s="5">
         <v>2804</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="37">
         <v>0</v>
       </c>
     </row>
@@ -8521,12 +8998,12 @@
       <c r="C7" s="5">
         <v>4102</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>65</v>
       </c>
       <c r="B8" s="5">
@@ -8535,12 +9012,12 @@
       <c r="C8" s="5">
         <v>2029</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="38">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>66</v>
       </c>
       <c r="B9" s="5">
@@ -8554,7 +9031,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>67</v>
       </c>
       <c r="B10" s="5">
@@ -8568,7 +9045,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>68</v>
       </c>
       <c r="B11" s="5">
@@ -8582,7 +9059,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>69</v>
       </c>
       <c r="B12" s="5">
@@ -8596,7 +9073,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>70</v>
       </c>
       <c r="B13" s="5">
@@ -8610,7 +9087,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>71</v>
       </c>
       <c r="B14" s="5">
@@ -8624,7 +9101,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>72</v>
       </c>
       <c r="B15" s="5">
@@ -8638,7 +9115,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="7">
         <v>73</v>
       </c>
       <c r="B16" s="5">
@@ -8652,7 +9129,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="7">
         <v>74</v>
       </c>
       <c r="B17" s="5">
@@ -8661,12 +9138,12 @@
       <c r="C17" s="5">
         <v>0</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="36">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="7">
         <v>75</v>
       </c>
       <c r="B18" s="5">
@@ -8679,51 +9156,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>95</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>3</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
       </c>
       <c r="C24" s="6">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="D24" s="6">
         <v>0</v>
@@ -8731,13 +9194,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="6">
         <v>0</v>
       </c>
       <c r="C25" s="6">
-        <v>308</v>
+        <v>37</v>
       </c>
       <c r="D25" s="6">
         <v>0</v>
@@ -8745,13 +9208,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C26" s="6">
-        <v>1212</v>
+        <v>308</v>
       </c>
       <c r="D26" s="6">
         <v>0</v>
@@ -8759,13 +9222,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="6">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C27" s="6">
-        <v>2565</v>
+        <v>1212</v>
       </c>
       <c r="D27" s="6">
         <v>0</v>
@@ -8773,13 +9236,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="6">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="C28" s="6">
-        <v>3046</v>
+        <v>2565</v>
       </c>
       <c r="D28" s="6">
         <v>0</v>
@@ -8787,147 +9250,147 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="6">
-        <v>774</v>
+        <v>200</v>
       </c>
       <c r="C29" s="6">
-        <v>1908</v>
+        <v>3046</v>
       </c>
       <c r="D29" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="6">
-        <v>1706</v>
+        <v>774</v>
       </c>
       <c r="C30" s="6">
-        <v>742</v>
+        <v>1908</v>
       </c>
       <c r="D30" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="6">
-        <v>2571</v>
+        <v>1706</v>
       </c>
       <c r="C31" s="6">
-        <v>152</v>
+        <v>742</v>
       </c>
       <c r="D31" s="6">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="6">
-        <v>2442</v>
+        <v>2571</v>
       </c>
       <c r="C32" s="6">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="D32" s="6">
-        <v>185</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="6">
-        <v>1473</v>
+        <v>2442</v>
       </c>
       <c r="C33" s="6">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D33" s="6">
-        <v>726</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" s="6">
-        <v>610</v>
+        <v>1473</v>
       </c>
       <c r="C34" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D34" s="6">
-        <v>1563</v>
+        <v>726</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35" s="6">
-        <v>152</v>
+        <v>610</v>
       </c>
       <c r="C35" s="6">
         <v>0</v>
       </c>
       <c r="D35" s="6">
-        <v>2396</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" s="6">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="C36" s="6">
         <v>0</v>
       </c>
       <c r="D36" s="6">
-        <v>2474</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="6">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C37" s="6">
         <v>0</v>
       </c>
       <c r="D37" s="6">
-        <v>1592</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C38" s="6">
         <v>0</v>
       </c>
       <c r="D38" s="6">
-        <v>742</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="6">
         <v>0</v>
@@ -8936,12 +9399,12 @@
         <v>0</v>
       </c>
       <c r="D39" s="6">
-        <v>220</v>
+        <v>742</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" s="6">
         <v>0</v>
@@ -8950,12 +9413,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="6">
-        <v>47</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" s="6">
         <v>0</v>
@@ -8964,12 +9427,12 @@
         <v>0</v>
       </c>
       <c r="D41" s="6">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="6">
         <v>0</v>
@@ -8978,68 +9441,54 @@
         <v>0</v>
       </c>
       <c r="D42" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>114</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0</v>
+      </c>
+      <c r="D43" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>192</v>
-      </c>
-      <c r="B46" s="6">
-        <v>0</v>
-      </c>
-      <c r="C46" s="6">
-        <v>3</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>193</v>
-      </c>
-      <c r="B47" s="6">
-        <v>0</v>
-      </c>
-      <c r="C47" s="6">
-        <v>7</v>
-      </c>
-      <c r="D47" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B48" s="6">
         <v>0</v>
       </c>
       <c r="C48" s="6">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
@@ -9047,13 +9496,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="6">
-        <v>177</v>
+        <v>3</v>
       </c>
       <c r="D49" s="6">
         <v>0</v>
@@ -9061,13 +9510,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B50" s="6">
         <v>0</v>
       </c>
       <c r="C50" s="6">
-        <v>494</v>
+        <v>7</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -9075,13 +9524,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="6">
-        <v>983</v>
+        <v>65</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
@@ -9089,13 +9538,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B52" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C52" s="6">
-        <v>1487</v>
+        <v>177</v>
       </c>
       <c r="D52" s="6">
         <v>0</v>
@@ -9103,13 +9552,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B53" s="6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C53" s="6">
-        <v>1812</v>
+        <v>494</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
@@ -9117,13 +9566,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B54" s="6">
-        <v>47</v>
-      </c>
-      <c r="C54" s="6">
-        <v>1846</v>
+        <v>1</v>
+      </c>
+      <c r="C54" s="39">
+        <v>983</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
@@ -9131,13 +9580,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B55" s="6">
-        <v>134</v>
+        <v>3</v>
       </c>
       <c r="C55" s="6">
-        <v>1463</v>
+        <v>1487</v>
       </c>
       <c r="D55" s="6">
         <v>0</v>
@@ -9145,13 +9594,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B56" s="6">
-        <v>261</v>
+        <v>17</v>
       </c>
       <c r="C56" s="6">
-        <v>940</v>
+        <v>1812</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
@@ -9159,13 +9608,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B57" s="6">
-        <v>507</v>
+        <v>47</v>
       </c>
       <c r="C57" s="6">
-        <v>445</v>
+        <v>1846</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
@@ -9173,231 +9622,231 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B58" s="6">
-        <v>883</v>
+        <v>134</v>
       </c>
       <c r="C58" s="6">
-        <v>198</v>
+        <v>1463</v>
       </c>
       <c r="D58" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B59" s="6">
-        <v>1210</v>
+        <v>261</v>
       </c>
       <c r="C59" s="6">
-        <v>59</v>
+        <v>940</v>
       </c>
       <c r="D59" s="6">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B60" s="6">
-        <v>1471</v>
+        <v>507</v>
       </c>
       <c r="C60" s="6">
-        <v>15</v>
+        <v>445</v>
       </c>
       <c r="D60" s="6">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B61" s="6">
-        <v>1532</v>
+        <v>883</v>
       </c>
       <c r="C61" s="6">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="D61" s="6">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B62" s="6">
-        <v>1369</v>
+        <v>1210</v>
       </c>
       <c r="C62" s="6">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="D62" s="6">
-        <v>278</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B63" s="6">
-        <v>1090</v>
+        <v>1471</v>
       </c>
       <c r="C63" s="6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D63" s="6">
-        <v>527</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B64" s="6">
-        <v>716</v>
+        <v>1532</v>
       </c>
       <c r="C64" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D64" s="6">
-        <v>893</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B65" s="6">
-        <v>410</v>
+        <v>1369</v>
       </c>
       <c r="C65" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="6">
-        <v>1226</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B66" s="6">
-        <v>211</v>
+        <v>1090</v>
       </c>
       <c r="C66" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="6">
-        <v>1582</v>
+        <v>527</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B67" s="6">
-        <v>81</v>
+        <v>716</v>
       </c>
       <c r="C67" s="6">
         <v>0</v>
       </c>
       <c r="D67" s="6">
-        <v>1581</v>
+        <v>893</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B68" s="6">
-        <v>44</v>
+        <v>410</v>
       </c>
       <c r="C68" s="6">
         <v>0</v>
       </c>
       <c r="D68" s="6">
-        <v>1445</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B69" s="6">
-        <v>10</v>
+        <v>211</v>
       </c>
       <c r="C69" s="6">
         <v>0</v>
       </c>
       <c r="D69" s="6">
-        <v>1017</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B70" s="6">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="C70" s="6">
         <v>0</v>
       </c>
       <c r="D70" s="6">
-        <v>665</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B71" s="6">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C71" s="6">
         <v>0</v>
       </c>
       <c r="D71" s="6">
-        <v>380</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B72" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C72" s="6">
         <v>0</v>
       </c>
       <c r="D72" s="6">
-        <v>156</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B73" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C73" s="6">
         <v>0</v>
       </c>
       <c r="D73" s="6">
-        <v>53</v>
+        <v>665</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B74" s="6">
         <v>0</v>
@@ -9406,12 +9855,12 @@
         <v>0</v>
       </c>
       <c r="D74" s="6">
-        <v>19</v>
+        <v>380</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B75" s="6">
         <v>0</v>
@@ -9420,12 +9869,12 @@
         <v>0</v>
       </c>
       <c r="D75" s="6">
-        <v>6</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B76" s="6">
         <v>0</v>
@@ -9434,304 +9883,418 @@
         <v>0</v>
       </c>
       <c r="D76" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>220</v>
+      </c>
+      <c r="B77" s="6">
+        <v>0</v>
+      </c>
+      <c r="C77" s="6">
+        <v>0</v>
+      </c>
+      <c r="D77" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>221</v>
+      </c>
+      <c r="B78" s="6">
+        <v>0</v>
+      </c>
+      <c r="C78" s="6">
+        <v>0</v>
+      </c>
+      <c r="D78" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>222</v>
+      </c>
+      <c r="B79" s="6">
+        <v>0</v>
+      </c>
+      <c r="C79" s="6">
+        <v>0</v>
+      </c>
+      <c r="D79" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="11"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="11"/>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="11"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="11"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="27" t="s">
+      <c r="A80" s="4">
+        <v>223</v>
+      </c>
+      <c r="B80" s="6">
+        <v>0</v>
+      </c>
+      <c r="C80" s="6">
+        <v>0</v>
+      </c>
+      <c r="D80" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>224</v>
+      </c>
+      <c r="B81" s="6">
+        <v>0</v>
+      </c>
+      <c r="C81" s="6">
+        <v>0</v>
+      </c>
+      <c r="D81" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>225</v>
+      </c>
+      <c r="B82" s="6">
+        <v>0</v>
+      </c>
+      <c r="C82" s="6">
+        <v>0</v>
+      </c>
+      <c r="D82" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>226</v>
+      </c>
+      <c r="B83" s="6">
+        <v>0</v>
+      </c>
+      <c r="C83" s="6">
+        <v>0</v>
+      </c>
+      <c r="D83" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>227</v>
+      </c>
+      <c r="B84" s="6">
+        <v>0</v>
+      </c>
+      <c r="C84" s="6">
+        <v>0</v>
+      </c>
+      <c r="D84" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="10"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="10"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="8"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="29"/>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
+      <c r="B91" s="28"/>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B92" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="13">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="12">
         <v>334</v>
       </c>
-      <c r="B85" s="14">
+      <c r="B93" s="13">
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="13">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="12">
         <v>335</v>
       </c>
-      <c r="B86" s="15">
+      <c r="B94" s="14">
         <v>455</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="13">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="12">
         <v>336</v>
       </c>
-      <c r="B87" s="15">
+      <c r="B95" s="14">
         <v>1455</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="13">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="12">
         <v>337</v>
       </c>
-      <c r="B88" s="15">
+      <c r="B96" s="14">
         <v>2061</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="13">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="12">
         <v>338</v>
       </c>
-      <c r="B89" s="15">
+      <c r="B97" s="14">
         <v>2051</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="13">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="12">
         <v>339</v>
       </c>
-      <c r="B90" s="15">
+      <c r="B98" s="14">
         <v>1522</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="13">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="12">
         <v>340</v>
       </c>
-      <c r="B91" s="15">
+      <c r="B99" s="14">
         <v>1076</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="13">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="12">
         <v>341</v>
       </c>
-      <c r="B92" s="15">
+      <c r="B100" s="14">
         <v>630</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="13">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="12">
         <v>342</v>
       </c>
-      <c r="B93" s="15">
+      <c r="B101" s="14">
         <v>343</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="13">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="12">
         <v>343</v>
       </c>
-      <c r="B94" s="15">
+      <c r="B102" s="14">
         <v>204</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="13">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="12">
         <v>344</v>
       </c>
-      <c r="B95" s="15">
+      <c r="B103" s="14">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="13">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="12">
         <v>345</v>
       </c>
-      <c r="B96" s="15">
+      <c r="B104" s="14">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="13">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="12">
         <v>346</v>
       </c>
-      <c r="B97" s="15">
+      <c r="B105" s="14">
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="13">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="12">
         <v>347</v>
       </c>
-      <c r="B98" s="15">
+      <c r="B106" s="14">
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="16">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="15">
         <v>348</v>
       </c>
-      <c r="B99" s="17">
+      <c r="B107" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="27" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B102" s="29"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="B110" s="28"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="13">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="12">
         <v>500</v>
       </c>
-      <c r="B104" s="18">
+      <c r="B112" s="17">
         <v>279</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="13">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="12">
         <v>501</v>
       </c>
-      <c r="B105" s="19">
+      <c r="B113" s="18">
         <v>2102</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="13">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="12">
         <v>502</v>
       </c>
-      <c r="B106" s="19">
+      <c r="B114" s="18">
         <v>2635</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="13">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="12">
         <v>503</v>
       </c>
-      <c r="B107" s="15">
+      <c r="B115" s="14">
         <v>2165</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="13">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="12">
         <v>504</v>
       </c>
-      <c r="B108" s="15">
+      <c r="B116" s="14">
         <v>1346</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="13">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="12">
         <v>505</v>
       </c>
-      <c r="B109" s="15">
+      <c r="B117" s="14">
         <v>782</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="13">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="12">
         <v>506</v>
       </c>
-      <c r="B110" s="15">
+      <c r="B118" s="14">
         <v>380</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="13">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="12">
         <v>507</v>
       </c>
-      <c r="B111" s="15">
+      <c r="B119" s="14">
         <v>176</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="13">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="12">
         <v>508</v>
       </c>
-      <c r="B112" s="15">
+      <c r="B120" s="14">
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="20">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="19">
         <v>509</v>
       </c>
-      <c r="B113" s="19">
+      <c r="B121" s="18">
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="20">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="19">
         <v>510</v>
       </c>
-      <c r="B114" s="19">
+      <c r="B122" s="18">
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="20">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="19">
         <v>511</v>
       </c>
-      <c r="B115" s="19">
+      <c r="B123" s="18">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="20">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="19">
         <v>512</v>
       </c>
-      <c r="B116" s="19">
+      <c r="B124" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="21">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="20">
         <v>513</v>
       </c>
-      <c r="B117" s="22">
+      <c r="B125" s="21">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A110:B110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9739,8 +10302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9751,16 +10314,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33"/>
+      <c r="B1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -9772,46 +10335,46 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>63</v>
       </c>
-      <c r="C3" s="26">
-        <v>13</v>
+      <c r="C3" s="25">
+        <v>703</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="24">
         <v>60</v>
       </c>
-      <c r="C4" s="25">
-        <v>6370</v>
+      <c r="C4" s="24">
+        <v>995</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23">
-        <v>65</v>
-      </c>
-      <c r="C5" s="24">
-        <v>1021</v>
+      <c r="B5" s="22">
+        <v>68</v>
+      </c>
+      <c r="C5" s="23">
+        <v>1062</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="32"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -9823,46 +10386,46 @@
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>98</v>
       </c>
-      <c r="C10" s="24">
-        <v>2364</v>
+      <c r="C10" s="23">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>95</v>
       </c>
-      <c r="C11" s="25">
-        <v>2077</v>
+      <c r="C11" s="24">
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>101</v>
       </c>
-      <c r="C12" s="24">
-        <v>7853</v>
+      <c r="C12" s="23">
+        <v>7999</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="33"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="B15" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="32"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -9874,29 +10437,29 @@
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="43">
         <v>197</v>
       </c>
-      <c r="C17" s="24">
-        <v>8357</v>
+      <c r="C17" s="40">
+        <v>704</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="41">
         <v>192</v>
       </c>
-      <c r="C18" s="25">
-        <v>1255</v>
+      <c r="C18" s="42">
+        <v>994</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="44">
         <v>204</v>
       </c>
       <c r="C19" s="24">
@@ -9904,16 +10467,16 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="32"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
@@ -9925,24 +10488,24 @@
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>334</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="32"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
@@ -9954,10 +10517,10 @@
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>500</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="23">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agrego el de 0.5
</commit_message>
<xml_diff>
--- a/Documentacion/GraficosGrafos.xlsx
+++ b/Documentacion/GraficosGrafos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,14 +79,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -302,21 +294,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -387,11 +364,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,29 +408,41 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -466,25 +475,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2660,499 +2666,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Grafo Regular 50% de Adyacencia</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[1]Graficos con porcentajes'!$B$89</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Coloreo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]Graficos con porcentajes'!$A$90:$A$104</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>335</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>338</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>339</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>341</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>342</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>344</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>345</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>346</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>347</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>348</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]Graficos con porcentajes'!$B$90:$B$104</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1455</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2061</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2051</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1522</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1076</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>630</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DA62-4D5E-878B-37FC96E29F29}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="422714335"/>
-        <c:axId val="417874959"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="422714335"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-ES"/>
-                  <a:t>Cantidad de colores</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="417874959"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="417874959"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-ES"/>
-                  <a:t>Frecuencia</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-AR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="422714335"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
               <a:t>Grafo Regular 75% de Adyacencia</a:t>
             </a:r>
           </a:p>
@@ -3605,7 +3118,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -3645,7 +3158,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4190,7 +3702,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4311,7 +3822,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4379,6 +3889,1068 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Grafo Regular 75% de Adyacencia</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Numero de corridas minimo'!$B$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Secuencial Aleatorio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Numero de corridas minimo'!$B$93:$B$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>974</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1755</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1833</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1330</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5825-4054-BE23-49D956FAFD37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Numero de corridas minimo'!$C$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wellsh Powell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Numero de corridas minimo'!$C$93:$C$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>943</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5825-4054-BE23-49D956FAFD37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Numero de corridas minimo'!$D$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matula</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]Graficos con porcentajes'!$A$45:$A$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Numero de corridas minimo'!$D$93:$D$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1787</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>858</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5825-4054-BE23-49D956FAFD37}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="553795679"/>
+        <c:axId val="553796927"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="553795679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-AR" baseline="0"/>
+                  <a:t> de colores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553796927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="553796927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Freciencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="553795679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -6174,7 +6746,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6185,7 +6757,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -6198,7 +6770,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -6215,7 +6787,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -6231,7 +6803,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -6275,45 +6847,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6325,31 +6887,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -6453,14 +7013,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -6550,20 +7104,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -6576,6 +7130,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6607,7 +7172,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -6616,14 +7181,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -6677,14 +7241,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -7272,53 +7830,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>99332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>72118</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>167368</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>53068</xdr:rowOff>
+      <xdr:colOff>557893</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>175532</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7339,7 +7859,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7369,6 +7889,44 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>225878</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>106816</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
@@ -7391,194 +7949,6 @@
         <row r="2">
           <cell r="B2" t="str">
             <v>Secuencial Aleatorio</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Wellsh Powell</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Matula</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>61</v>
-          </cell>
-          <cell r="B3">
-            <v>0</v>
-          </cell>
-          <cell r="C3">
-            <v>63</v>
-          </cell>
-          <cell r="D3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>62</v>
-          </cell>
-          <cell r="B4">
-            <v>1</v>
-          </cell>
-          <cell r="C4">
-            <v>775</v>
-          </cell>
-          <cell r="D4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>63</v>
-          </cell>
-          <cell r="B5">
-            <v>12</v>
-          </cell>
-          <cell r="C5">
-            <v>2967</v>
-          </cell>
-          <cell r="D5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>64</v>
-          </cell>
-          <cell r="B6">
-            <v>154</v>
-          </cell>
-          <cell r="C6">
-            <v>4003</v>
-          </cell>
-          <cell r="D6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>65</v>
-          </cell>
-          <cell r="B7">
-            <v>965</v>
-          </cell>
-          <cell r="C7">
-            <v>1860</v>
-          </cell>
-          <cell r="D7">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>66</v>
-          </cell>
-          <cell r="B8">
-            <v>2778</v>
-          </cell>
-          <cell r="C8">
-            <v>310</v>
-          </cell>
-          <cell r="D8">
-            <v>44</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>67</v>
-          </cell>
-          <cell r="B9">
-            <v>3522</v>
-          </cell>
-          <cell r="C9">
-            <v>22</v>
-          </cell>
-          <cell r="D9">
-            <v>419</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>68</v>
-          </cell>
-          <cell r="B10">
-            <v>2024</v>
-          </cell>
-          <cell r="C10">
-            <v>0</v>
-          </cell>
-          <cell r="D10">
-            <v>1903</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>69</v>
-          </cell>
-          <cell r="B11">
-            <v>481</v>
-          </cell>
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-          <cell r="D11">
-            <v>3494</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>70</v>
-          </cell>
-          <cell r="B12">
-            <v>57</v>
-          </cell>
-          <cell r="C12">
-            <v>0</v>
-          </cell>
-          <cell r="D12">
-            <v>2912</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>71</v>
-          </cell>
-          <cell r="B13">
-            <v>6</v>
-          </cell>
-          <cell r="C13">
-            <v>0</v>
-          </cell>
-          <cell r="D13">
-            <v>1006</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>72</v>
-          </cell>
-          <cell r="B14">
-            <v>0</v>
-          </cell>
-          <cell r="C14">
-            <v>0</v>
-          </cell>
-          <cell r="D14">
-            <v>202</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>73</v>
-          </cell>
-          <cell r="B15">
-            <v>0</v>
-          </cell>
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-          <cell r="D15">
-            <v>18</v>
           </cell>
         </row>
         <row r="21">
@@ -8896,10 +9266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D125"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8911,12 +9281,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -8942,7 +9312,7 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="23">
         <v>0</v>
       </c>
     </row>
@@ -8956,7 +9326,7 @@
       <c r="C4" s="5">
         <v>52</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="23">
         <v>0</v>
       </c>
     </row>
@@ -8970,7 +9340,7 @@
       <c r="C5" s="5">
         <v>647</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="23">
         <v>0</v>
       </c>
     </row>
@@ -8984,7 +9354,7 @@
       <c r="C6" s="5">
         <v>2804</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="23">
         <v>0</v>
       </c>
     </row>
@@ -8998,7 +9368,7 @@
       <c r="C7" s="5">
         <v>4102</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9012,7 +9382,7 @@
       <c r="C8" s="5">
         <v>2029</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="24">
         <v>1</v>
       </c>
     </row>
@@ -9138,7 +9508,7 @@
       <c r="C17" s="5">
         <v>0</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="22">
         <v>4</v>
       </c>
     </row>
@@ -9157,12 +9527,12 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -9459,12 +9829,12 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="28"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -9482,13 +9852,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B48" s="6">
         <v>0</v>
       </c>
       <c r="C48" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
@@ -9496,13 +9866,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D49" s="6">
         <v>0</v>
@@ -9510,13 +9880,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" s="6">
         <v>0</v>
       </c>
       <c r="C50" s="6">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -9524,13 +9894,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B51" s="6">
         <v>0</v>
       </c>
       <c r="C51" s="6">
-        <v>65</v>
+        <v>177</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
@@ -9538,13 +9908,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" s="6">
         <v>0</v>
       </c>
       <c r="C52" s="6">
-        <v>177</v>
+        <v>494</v>
       </c>
       <c r="D52" s="6">
         <v>0</v>
@@ -9552,13 +9922,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B53" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="6">
-        <v>494</v>
+        <v>983</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
@@ -9566,13 +9936,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B54" s="6">
-        <v>1</v>
-      </c>
-      <c r="C54" s="39">
-        <v>983</v>
+        <v>3</v>
+      </c>
+      <c r="C54" s="25">
+        <v>1487</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
@@ -9580,13 +9950,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B55" s="6">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C55" s="6">
-        <v>1487</v>
+        <v>1812</v>
       </c>
       <c r="D55" s="6">
         <v>0</v>
@@ -9594,13 +9964,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B56" s="6">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C56" s="6">
-        <v>1812</v>
+        <v>1846</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
@@ -9608,13 +9978,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B57" s="6">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="C57" s="6">
-        <v>1846</v>
+        <v>1463</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
@@ -9622,13 +9992,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B58" s="6">
-        <v>134</v>
+        <v>261</v>
       </c>
       <c r="C58" s="6">
-        <v>1463</v>
+        <v>940</v>
       </c>
       <c r="D58" s="6">
         <v>0</v>
@@ -9636,13 +10006,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B59" s="6">
-        <v>261</v>
+        <v>507</v>
       </c>
       <c r="C59" s="6">
-        <v>940</v>
+        <v>445</v>
       </c>
       <c r="D59" s="6">
         <v>0</v>
@@ -9650,203 +10020,203 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B60" s="6">
-        <v>507</v>
+        <v>883</v>
       </c>
       <c r="C60" s="6">
-        <v>445</v>
+        <v>198</v>
       </c>
       <c r="D60" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B61" s="6">
-        <v>883</v>
+        <v>1210</v>
       </c>
       <c r="C61" s="6">
-        <v>198</v>
+        <v>59</v>
       </c>
       <c r="D61" s="6">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B62" s="6">
-        <v>1210</v>
+        <v>1471</v>
       </c>
       <c r="C62" s="6">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D62" s="6">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B63" s="6">
-        <v>1471</v>
+        <v>1532</v>
       </c>
       <c r="C63" s="6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D63" s="6">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B64" s="6">
-        <v>1532</v>
+        <v>1369</v>
       </c>
       <c r="C64" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D64" s="6">
-        <v>95</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B65" s="6">
-        <v>1369</v>
+        <v>1090</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
       </c>
       <c r="D65" s="6">
-        <v>278</v>
+        <v>527</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B66" s="6">
-        <v>1090</v>
+        <v>716</v>
       </c>
       <c r="C66" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" s="6">
-        <v>527</v>
+        <v>893</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B67" s="6">
-        <v>716</v>
+        <v>410</v>
       </c>
       <c r="C67" s="6">
         <v>0</v>
       </c>
       <c r="D67" s="6">
-        <v>893</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
+        <v>212</v>
+      </c>
+      <c r="B68" s="6">
         <v>211</v>
-      </c>
-      <c r="B68" s="6">
-        <v>410</v>
       </c>
       <c r="C68" s="6">
         <v>0</v>
       </c>
       <c r="D68" s="6">
-        <v>1226</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B69" s="6">
-        <v>211</v>
+        <v>81</v>
       </c>
       <c r="C69" s="6">
         <v>0</v>
       </c>
       <c r="D69" s="6">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B70" s="6">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C70" s="6">
         <v>0</v>
       </c>
       <c r="D70" s="6">
-        <v>1581</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B71" s="6">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C71" s="6">
         <v>0</v>
       </c>
       <c r="D71" s="6">
-        <v>1445</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B72" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C72" s="6">
         <v>0</v>
       </c>
       <c r="D72" s="6">
-        <v>1017</v>
+        <v>665</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B73" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C73" s="6">
         <v>0</v>
       </c>
       <c r="D73" s="6">
-        <v>665</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B74" s="6">
         <v>0</v>
@@ -9855,12 +10225,12 @@
         <v>0</v>
       </c>
       <c r="D74" s="6">
-        <v>380</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B75" s="6">
         <v>0</v>
@@ -9869,12 +10239,12 @@
         <v>0</v>
       </c>
       <c r="D75" s="6">
-        <v>156</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B76" s="6">
         <v>0</v>
@@ -9883,12 +10253,12 @@
         <v>0</v>
       </c>
       <c r="D76" s="6">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B77" s="6">
         <v>0</v>
@@ -9897,12 +10267,12 @@
         <v>0</v>
       </c>
       <c r="D77" s="6">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B78" s="6">
         <v>0</v>
@@ -9911,7 +10281,7 @@
         <v>0</v>
       </c>
       <c r="D78" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -10025,262 +10395,416 @@
       <c r="C89" s="10"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="28"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+      <c r="B91" s="41"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="41"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>334</v>
+      </c>
+      <c r="B93" s="6">
+        <v>10</v>
+      </c>
+      <c r="C93" s="6">
+        <v>9</v>
+      </c>
+      <c r="D93" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>335</v>
+      </c>
+      <c r="B94" s="6">
+        <v>216</v>
+      </c>
+      <c r="C94" s="6">
+        <v>198</v>
+      </c>
+      <c r="D94" s="6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>336</v>
+      </c>
+      <c r="B95" s="6">
+        <v>974</v>
+      </c>
+      <c r="C95" s="6">
+        <v>943</v>
+      </c>
+      <c r="D95" s="6">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>337</v>
+      </c>
+      <c r="B96" s="6">
+        <v>1755</v>
+      </c>
+      <c r="C96" s="6">
+        <v>1817</v>
+      </c>
+      <c r="D96" s="6">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>338</v>
+      </c>
+      <c r="B97" s="6">
+        <v>2021</v>
+      </c>
+      <c r="C97" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D97" s="6">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>339</v>
+      </c>
+      <c r="B98" s="6">
+        <v>1833</v>
+      </c>
+      <c r="C98" s="6">
+        <v>1844</v>
+      </c>
+      <c r="D98" s="6">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>340</v>
+      </c>
+      <c r="B99" s="6">
+        <v>1330</v>
+      </c>
+      <c r="C99" s="6">
+        <v>1308</v>
+      </c>
+      <c r="D99" s="6">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>341</v>
+      </c>
+      <c r="B100" s="6">
+        <v>848</v>
+      </c>
+      <c r="C100" s="6">
+        <v>859</v>
+      </c>
+      <c r="D100" s="6">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>342</v>
+      </c>
+      <c r="B101" s="6">
+        <v>495</v>
+      </c>
+      <c r="C101" s="6">
+        <v>507</v>
+      </c>
+      <c r="D101" s="6">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>343</v>
+      </c>
+      <c r="B102" s="6">
+        <v>264</v>
+      </c>
+      <c r="C102" s="6">
+        <v>258</v>
+      </c>
+      <c r="D102" s="6">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>344</v>
+      </c>
+      <c r="B103" s="6">
+        <v>129</v>
+      </c>
+      <c r="C103" s="6">
+        <v>138</v>
+      </c>
+      <c r="D103" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>345</v>
+      </c>
+      <c r="B104" s="6">
+        <v>71</v>
+      </c>
+      <c r="C104" s="6">
+        <v>54</v>
+      </c>
+      <c r="D104" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>346</v>
+      </c>
+      <c r="B105" s="6">
+        <v>30</v>
+      </c>
+      <c r="C105" s="6">
+        <v>33</v>
+      </c>
+      <c r="D105" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>347</v>
+      </c>
+      <c r="B106" s="6">
+        <v>17</v>
+      </c>
+      <c r="C106" s="6">
+        <v>13</v>
+      </c>
+      <c r="D106" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>348</v>
+      </c>
+      <c r="B107" s="6">
+        <v>3</v>
+      </c>
+      <c r="C107" s="6">
+        <v>3</v>
+      </c>
+      <c r="D107" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>349</v>
+      </c>
+      <c r="B108" s="6">
+        <v>2</v>
+      </c>
+      <c r="C108" s="6">
+        <v>0</v>
+      </c>
+      <c r="D108" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="6">
+        <v>350</v>
+      </c>
+      <c r="B109" s="6">
+        <v>1</v>
+      </c>
+      <c r="C109" s="6">
+        <v>1</v>
+      </c>
+      <c r="D109" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="6">
+        <v>351</v>
+      </c>
+      <c r="B110" s="6">
+        <v>1</v>
+      </c>
+      <c r="C110" s="6">
+        <v>0</v>
+      </c>
+      <c r="D110" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="6">
+        <v>352</v>
+      </c>
+      <c r="B111" s="6">
+        <v>0</v>
+      </c>
+      <c r="C111" s="6">
+        <v>0</v>
+      </c>
+      <c r="D111" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135" s="32"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="12">
-        <v>334</v>
-      </c>
-      <c r="B93" s="13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="12">
-        <v>335</v>
-      </c>
-      <c r="B94" s="14">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="12">
-        <v>336</v>
-      </c>
-      <c r="B95" s="14">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="12">
-        <v>337</v>
-      </c>
-      <c r="B96" s="14">
-        <v>2061</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="12">
-        <v>338</v>
-      </c>
-      <c r="B97" s="14">
-        <v>2051</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="12">
-        <v>339</v>
-      </c>
-      <c r="B98" s="14">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="12">
-        <v>340</v>
-      </c>
-      <c r="B99" s="14">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="12">
-        <v>341</v>
-      </c>
-      <c r="B100" s="14">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="12">
-        <v>342</v>
-      </c>
-      <c r="B101" s="14">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="12">
-        <v>343</v>
-      </c>
-      <c r="B102" s="14">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="12">
-        <v>344</v>
-      </c>
-      <c r="B103" s="14">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="12">
-        <v>345</v>
-      </c>
-      <c r="B104" s="14">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="12">
-        <v>346</v>
-      </c>
-      <c r="B105" s="14">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="12">
-        <v>347</v>
-      </c>
-      <c r="B106" s="14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="15">
-        <v>348</v>
-      </c>
-      <c r="B107" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B110" s="28"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="11">
+        <v>500</v>
+      </c>
+      <c r="B137" s="13">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="11">
+        <v>501</v>
+      </c>
+      <c r="B138" s="14">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="11">
+        <v>502</v>
+      </c>
+      <c r="B139" s="14">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="11">
+        <v>503</v>
+      </c>
+      <c r="B140" s="12">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="11">
+        <v>504</v>
+      </c>
+      <c r="B141" s="12">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="11">
+        <v>505</v>
+      </c>
+      <c r="B142" s="12">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="11">
+        <v>506</v>
+      </c>
+      <c r="B143" s="12">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="11">
+        <v>507</v>
+      </c>
+      <c r="B144" s="12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="11">
+        <v>508</v>
+      </c>
+      <c r="B145" s="12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="15">
+        <v>509</v>
+      </c>
+      <c r="B146" s="14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="15">
+        <v>510</v>
+      </c>
+      <c r="B147" s="14">
         <v>11</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="12">
-        <v>500</v>
-      </c>
-      <c r="B112" s="17">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="12">
-        <v>501</v>
-      </c>
-      <c r="B113" s="18">
-        <v>2102</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="12">
-        <v>502</v>
-      </c>
-      <c r="B114" s="18">
-        <v>2635</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="12">
-        <v>503</v>
-      </c>
-      <c r="B115" s="14">
-        <v>2165</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="12">
-        <v>504</v>
-      </c>
-      <c r="B116" s="14">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="12">
-        <v>505</v>
-      </c>
-      <c r="B117" s="14">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="12">
-        <v>506</v>
-      </c>
-      <c r="B118" s="14">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="12">
-        <v>507</v>
-      </c>
-      <c r="B119" s="14">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="12">
-        <v>508</v>
-      </c>
-      <c r="B120" s="14">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="19">
-        <v>509</v>
-      </c>
-      <c r="B121" s="18">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="19">
-        <v>510</v>
-      </c>
-      <c r="B122" s="18">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="19">
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="15">
         <v>511</v>
       </c>
-      <c r="B123" s="18">
+      <c r="B148" s="14">
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="19">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="15">
         <v>512</v>
       </c>
-      <c r="B124" s="18">
+      <c r="B149" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="20">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="16">
         <v>513</v>
       </c>
-      <c r="B125" s="21">
+      <c r="B150" s="17">
         <v>1</v>
       </c>
     </row>
@@ -10289,8 +10813,8 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A91:D91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10300,10 +10824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10314,16 +10838,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
+      <c r="A2" s="38"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -10335,10 +10859,10 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="18">
         <v>63</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="21">
         <v>703</v>
       </c>
     </row>
@@ -10346,10 +10870,10 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="20">
         <v>60</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="20">
         <v>995</v>
       </c>
     </row>
@@ -10357,24 +10881,24 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="18">
         <v>68</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="19">
         <v>1062</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="36"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -10386,10 +10910,10 @@
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="18">
         <v>98</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="19">
         <v>17</v>
       </c>
     </row>
@@ -10397,10 +10921,10 @@
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="18">
         <v>95</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="20">
         <v>441</v>
       </c>
     </row>
@@ -10408,24 +10932,24 @@
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="18">
         <v>101</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <v>7999</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -10437,10 +10961,10 @@
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43">
+      <c r="B17" s="28">
         <v>197</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="45">
         <v>704</v>
       </c>
     </row>
@@ -10448,10 +10972,10 @@
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="26">
         <v>192</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="27">
         <v>994</v>
       </c>
     </row>
@@ -10459,24 +10983,24 @@
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="29">
         <v>204</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="20">
         <v>1063</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="32"/>
+      <c r="C22" s="36"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
@@ -10488,48 +11012,97 @@
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="18">
         <v>334</v>
       </c>
-      <c r="C24" s="23">
-        <v>172</v>
+      <c r="C24" s="19">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="18">
+        <v>334</v>
+      </c>
+      <c r="C25" s="20">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="18">
+        <v>344</v>
+      </c>
+      <c r="C26" s="19">
+        <v>4973</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="42"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B28" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="36"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="38"/>
+      <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B30" s="18">
         <v>500</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C30" s="19">
         <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="18">
+        <v>95</v>
+      </c>
+      <c r="C31" s="20">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="18">
+        <v>101</v>
+      </c>
+      <c r="C32" s="19">
+        <v>7999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A8:A9"/>

</xml_diff>